<commit_message>
Corrected DailyTradingPlan currencies for non-US markets
</commit_message>
<xml_diff>
--- a/DailyTradingPlan_DE.xlsx
+++ b/DailyTradingPlan_DE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\PycharmProjects\ibbot100_data\MTA_GitHub\241005\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\PycharmProjects\Momentum-Trading-Assistant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1536688B-675C-4E1F-9577-2BACF9F808E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50758FC-DAA0-4846-AF5E-852AE976932B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
   <si>
     <t>Symbol</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>IBIS</t>
+  </si>
+  <si>
+    <t>EUR</t>
   </si>
 </sst>
 </file>
@@ -664,7 +667,7 @@
   <dimension ref="A1:CA290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1028,7 +1031,7 @@
         <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
@@ -1066,7 +1069,7 @@
         <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>

</xml_diff>